<commit_message>
For use_html5lib branch update. Still cannot retrieve Cash and Cash Equalivent. Commit the code to the branch for working from Toronto
</commit_message>
<xml_diff>
--- a/TD.TO.xlsx
+++ b/TD.TO.xlsx
@@ -478,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1106,9 +1106,18 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.002504177964019358</v>
+        <v>-0.002643222304835081</v>
       </c>
       <c r="C69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.003905687958732096</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>